<commit_message>
Fix Excel template and skip sample rows during import
Template improvements:
- Added color legend to Introduction sheet (yellow=dropdown, white=free text, grey=sample)
- Added legend reminder to row 4 of all data sheets
- Added grey sample data rows to all sheets (marked with "SAMPLE")

Parser fix:
- Skip rows containing "SAMPLE" or "EXAMPLE" during import
- These are template examples, not real data

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/climatrix_files/climatrix_import_template_scope1and2_v3.xlsx
+++ b/backend/climatrix_files/climatrix_import_template_scope1and2_v3.xlsx
@@ -25,7 +25,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -73,8 +73,12 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -99,6 +103,18 @@
         <bgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -118,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -137,6 +153,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -502,7 +527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +559,6 @@
         </is>
       </c>
     </row>
-    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -549,7 +573,6 @@
         </is>
       </c>
     </row>
-    <row r="9"/>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
@@ -563,7 +586,6 @@
         <v/>
       </c>
     </row>
-    <row r="12"/>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
@@ -592,7 +614,6 @@
         </is>
       </c>
     </row>
-    <row r="17"/>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
@@ -635,7 +656,6 @@
         </is>
       </c>
     </row>
-    <row r="24"/>
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
@@ -664,7 +684,6 @@
         </is>
       </c>
     </row>
-    <row r="29"/>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
@@ -686,7 +705,6 @@
         </is>
       </c>
     </row>
-    <row r="33"/>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
@@ -715,7 +733,6 @@
         </is>
       </c>
     </row>
-    <row r="38"/>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
@@ -744,7 +761,6 @@
         </is>
       </c>
     </row>
-    <row r="43"/>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
@@ -753,21 +769,36 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Save this file as .xlsx (Excel format)</t>
+      <c r="A45" s="14" t="inlineStr">
+        <is>
+          <t>COLOR LEGEND</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Upload to CLIMATERIX via Import page</t>
-        </is>
-      </c>
-    </row>
-    <row r="47"/>
-    <row r="48"/>
+      <c r="A46" s="15" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown (select from list)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="16" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>White = Free text (type your value)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="17" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Grey = Sample data (will be skipped during import)</t>
+        </is>
+      </c>
+    </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
@@ -781,7 +812,6 @@
         <v/>
       </c>
     </row>
-    <row r="51"/>
     <row r="52">
       <c r="A52" s="5" t="inlineStr">
         <is>
@@ -803,8 +833,6 @@
         </is>
       </c>
     </row>
-    <row r="55"/>
-    <row r="56"/>
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
@@ -818,7 +846,6 @@
         <v/>
       </c>
     </row>
-    <row r="59"/>
     <row r="60">
       <c r="A60" s="5" t="inlineStr">
         <is>
@@ -861,8 +888,6 @@
         </is>
       </c>
     </row>
-    <row r="66"/>
-    <row r="67"/>
     <row r="68">
       <c r="A68" s="4" t="inlineStr">
         <is>
@@ -876,7 +901,6 @@
         <v/>
       </c>
     </row>
-    <row r="70"/>
     <row r="71">
       <c r="A71" s="5" t="inlineStr">
         <is>
@@ -891,7 +915,6 @@
         </is>
       </c>
     </row>
-    <row r="73"/>
     <row r="76">
       <c r="A76" s="13" t="inlineStr">
         <is>
@@ -1105,7 +1128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1137,19 +1160,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Fuel Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -1183,37 +1206,37 @@
       <c r="G5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
         <is>
           <t>Natural Gas</t>
         </is>
       </c>
-      <c r="B6" s="12" t="inlineStr">
+      <c r="B6" s="19" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
-      <c r="C6" s="12" t="inlineStr">
-        <is>
-          <t>Office heating - Q1 2024</t>
-        </is>
-      </c>
-      <c r="D6" s="12" t="inlineStr">
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>Office heating - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
         <is>
           <t>15000</t>
         </is>
       </c>
-      <c r="E6" s="12" t="inlineStr">
+      <c r="E6" s="19" t="inlineStr">
         <is>
           <t>kWh</t>
         </is>
       </c>
-      <c r="F6" s="12" t="inlineStr">
+      <c r="F6" s="19" t="inlineStr">
         <is>
           <t>2024-01</t>
         </is>
       </c>
-      <c r="G6" s="12" t="inlineStr">
+      <c r="G6" s="19" t="inlineStr">
         <is>
           <t>HQ Building</t>
         </is>
@@ -2219,7 +2242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2251,19 +2274,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Vehicle Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Fuel Type</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -2297,41 +2320,37 @@
       <c r="G5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>Diesel</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
+        <is>
+          <t>Petrol</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
-      <c r="D6" s="12" t="inlineStr">
-        <is>
-          <t>Sales team vehicle ABC-123</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
-        <is>
-          <t>25000</t>
-        </is>
-      </c>
-      <c r="F6" s="12" t="inlineStr">
-        <is>
-          <t>km</t>
-        </is>
-      </c>
-      <c r="G6" s="12" t="inlineStr">
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>Company car - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
+        <is>
+          <t>liters</t>
+        </is>
+      </c>
+      <c r="F6" s="19" t="inlineStr">
         <is>
           <t>2024-01</t>
         </is>
       </c>
+      <c r="G6" s="19" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="inlineStr">
@@ -3373,7 +3392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3404,19 +3423,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Refrigerant Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -3444,34 +3463,35 @@
       <c r="F5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
         <is>
           <t>R-410A</t>
         </is>
       </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="inlineStr">
-        <is>
-          <t>AC system refill - Building A</t>
-        </is>
-      </c>
-      <c r="D6" s="12" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
+      <c r="B6" s="19" t="inlineStr"/>
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>AC top-up - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
         <is>
           <t>kg</t>
         </is>
       </c>
-      <c r="F6" s="12" t="inlineStr">
-        <is>
-          <t>2024-03</t>
+      <c r="F6" s="19" t="inlineStr">
+        <is>
+          <t>2024-01</t>
+        </is>
+      </c>
+      <c r="G6" s="20" t="inlineStr">
+        <is>
+          <t>Main Office</t>
         </is>
       </c>
     </row>
@@ -3933,7 +3953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3965,19 +3985,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Electricity Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Country/Region</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -4011,39 +4031,39 @@
       <c r="G5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>Grid Electricity (Location-based)</t>
-        </is>
-      </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="inlineStr">
-        <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="D6" s="12" t="inlineStr">
-        <is>
-          <t>Main office - Tel Aviv</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
-        <is>
-          <t>45000</t>
-        </is>
-      </c>
-      <c r="F6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
+        <is>
+          <t>IL - Israel</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>Monthly bill - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
         <is>
           <t>kWh</t>
         </is>
       </c>
-      <c r="G6" s="12" t="inlineStr">
+      <c r="F6" s="19" t="inlineStr">
         <is>
           <t>2024-01</t>
+        </is>
+      </c>
+      <c r="G6" s="19" t="inlineStr">
+        <is>
+          <t>HQ</t>
         </is>
       </c>
     </row>
@@ -5124,7 +5144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5155,19 +5175,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Energy Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -5195,36 +5215,33 @@
       <c r="F5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>District Heating</t>
-        </is>
-      </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="inlineStr">
-        <is>
-          <t>Office heating - Winter 2024</t>
-        </is>
-      </c>
-      <c r="D6" s="12" t="inlineStr">
-        <is>
-          <t>35000</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
+        <is>
+          <t>IL - Israel</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="inlineStr"/>
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>District heating - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
         <is>
           <t>kWh</t>
         </is>
       </c>
-      <c r="F6" s="12" t="inlineStr">
-        <is>
-          <t>2024-Q1</t>
-        </is>
-      </c>
+      <c r="F6" s="19" t="inlineStr">
+        <is>
+          <t>2024-01</t>
+        </is>
+      </c>
+      <c r="G6" s="20" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="inlineStr">
@@ -5716,7 +5733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5747,19 +5764,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Cooling Type</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C4" s="10" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="A4" s="18" t="inlineStr">
+        <is>
+          <t>Yellow = Dropdown</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="inlineStr">
+        <is>
+          <t>White = Free text</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
+        <is>
+          <t>Grey rows = Sample (skipped)</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -5787,36 +5804,33 @@
       <c r="F5" s="11" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t>Chilled Water</t>
-        </is>
-      </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C6" s="12" t="inlineStr">
-        <is>
-          <t>Data center cooling</t>
-        </is>
-      </c>
-      <c r="D6" s="12" t="inlineStr">
-        <is>
-          <t>42000</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
+      <c r="A6" s="19" t="inlineStr">
+        <is>
+          <t>IL - Israel</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="inlineStr"/>
+      <c r="C6" s="19" t="inlineStr">
+        <is>
+          <t>Cooling system - SAMPLE</t>
+        </is>
+      </c>
+      <c r="D6" s="19" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="E6" s="19" t="inlineStr">
         <is>
           <t>kWh</t>
         </is>
       </c>
-      <c r="F6" s="12" t="inlineStr">
-        <is>
-          <t>2024-02</t>
-        </is>
-      </c>
+      <c r="F6" s="19" t="inlineStr">
+        <is>
+          <t>2024-01</t>
+        </is>
+      </c>
+      <c r="G6" s="20" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="inlineStr">

</xml_diff>